<commit_message>
EPBDS-8247 Implement ability to store description of Conditions and Return and Input data separately from Rules table.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7806_SmartLookup_Horisontal_Conditions.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7806_SmartLookup_Horisontal_Conditions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878620A0-4F02-41F3-9C94-E5FEB46C6C78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +81,6 @@
     <t>own</t>
   </si>
   <si>
-    <t xml:space="preserve"> dAge</t>
-  </si>
-  <si>
     <t xml:space="preserve"> carBrand</t>
   </si>
   <si>
@@ -96,13 +99,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>SmartLookup Double DriverPremium (carAge cAge,carSize Size, carOwner own, Integer dAge, brand carBrand )</t>
+    <t>SmartLookup Double DriverPremium (carAge cAge,carSize Size, carOwner own, Integer driverAge, brand carBrand )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> driverAge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -217,10 +223,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -247,7 +252,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -256,14 +261,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -301,9 +309,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,9 +344,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,9 +396,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,11 +588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:N63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +606,7 @@
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1689,30 +1731,30 @@
         <v>18</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1838,7 +1880,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -1888,7 +1930,6 @@
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="7"/>
       <c r="F55" s="1">
         <v>15</v>
       </c>
@@ -1897,43 +1938,21 @@
       <c r="B56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="F57" s="7"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="7"/>
-      <c r="F58" s="7"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="7"/>
-      <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="7"/>
-      <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D61" s="7"/>
-      <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D62" s="7"/>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D63" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1965,7 +1984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1977,7 +1996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>